<commit_message>
updated visualization with pie charts
</commit_message>
<xml_diff>
--- a/results/gpt-single-domain-results.xlsx
+++ b/results/gpt-single-domain-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaarmstrong/Desktop/PycharmProjects/llm-only-context/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaarmstrong/Desktop/PycharmProjects/llms-for-additional-context-extraction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847727F-9229-F348-8E6C-F37829DC9011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35D5264-905D-8841-A002-16506DFCE3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2616,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>